<commit_message>
Update default enhancement settings
</commit_message>
<xml_diff>
--- a/assets/mhrise-buffs.xlsx
+++ b/assets/mhrise-buffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\yuzu\works\repo\mhrise-damage-simulator\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6023F78F-C07A-4528-B1B4-B22628AAE2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C93494-FC2A-4BB0-898C-B67126ADFAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="1755" windowWidth="38700" windowHeight="15345" xr2:uid="{FF78F63D-3AAE-493B-BBA9-05ACB18EEBBB}"/>
+    <workbookView xWindow="3885" yWindow="2055" windowWidth="38700" windowHeight="15345" xr2:uid="{FF78F63D-3AAE-493B-BBA9-05ACB18EEBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="mhrise-buffs" sheetId="1" r:id="rId1"/>
@@ -1855,10 +1855,10 @@
   <dimension ref="A1:R364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E260" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="J334" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K284" sqref="K284"/>
+      <selection pane="bottomRight" activeCell="Q363" sqref="Q363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -16829,7 +16829,7 @@
         <v>99</v>
       </c>
       <c r="Q292" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="293" spans="1:18" x14ac:dyDescent="0.4">
@@ -17868,7 +17868,7 @@
         <v>99</v>
       </c>
       <c r="Q313" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R313" s="3" t="s">
         <v>311</v>
@@ -18204,7 +18204,7 @@
         <v>99</v>
       </c>
       <c r="Q319" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R319" s="3" t="s">
         <v>311</v>
@@ -18540,7 +18540,7 @@
         <v>99</v>
       </c>
       <c r="Q325" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R325" s="3" t="s">
         <v>312</v>
@@ -18861,7 +18861,7 @@
         <v>99</v>
       </c>
       <c r="Q331" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="332" spans="1:18" x14ac:dyDescent="0.4">
@@ -19179,7 +19179,7 @@
         <v>99</v>
       </c>
       <c r="Q337" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="338" spans="1:17" x14ac:dyDescent="0.4">
@@ -19497,7 +19497,7 @@
         <v>99</v>
       </c>
       <c r="Q343" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="344" spans="1:17" x14ac:dyDescent="0.4">
@@ -19547,7 +19547,7 @@
         <v>99</v>
       </c>
       <c r="Q344" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="345" spans="1:17" x14ac:dyDescent="0.4">
@@ -20059,7 +20059,7 @@
         <v>99</v>
       </c>
       <c r="Q354" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="355" spans="1:17" x14ac:dyDescent="0.4">
@@ -20271,7 +20271,7 @@
         <v>99</v>
       </c>
       <c r="Q358" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="359" spans="1:17" x14ac:dyDescent="0.4">
@@ -20483,7 +20483,7 @@
         <v>99</v>
       </c>
       <c r="Q362" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="363" spans="1:17" x14ac:dyDescent="0.4">

</xml_diff>